<commit_message>
code fixes and updated packages to get to compile
</commit_message>
<xml_diff>
--- a/tree/master/cloud/src/deployments/MCDeploymentConfig.xlsx
+++ b/tree/master/cloud/src/deployments/MCDeploymentConfig.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\mc\tree\master\cloud\src\deployments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\Git\mattercenter\tree\master\cloud\src\deployments\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="62310" yWindow="0" windowWidth="24270" windowHeight="12270" tabRatio="822" activeTab="5"/>
+    <workbookView xWindow="62310" yWindow="0" windowWidth="24270" windowHeight="12270" tabRatio="822" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Read Me" sheetId="11" r:id="rId1"/>
@@ -353,96 +353,9 @@
     <t>User4;</t>
   </si>
   <si>
-    <r>
-      <t>https://</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;TENANTNAME&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.sharepoint.com</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>https://</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;TENANTNAME&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-admin.sharepoint.com</t>
-    </r>
-  </si>
-  <si>
-    <t>COMPLETE USER EMAIL ADDRESS e.g. useralias@domain.com or useralias@tenantname.onmicrosoft.com</t>
-  </si>
-  <si>
     <t>Emails; Documents</t>
   </si>
   <si>
-    <t>&lt;ClientName only e.g. Microsoft&gt;</t>
-  </si>
-  <si>
-    <r>
-      <t>https://</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;TENANTNAME&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.sharepoint.com/teams/&lt;ClientName&gt;</t>
-    </r>
-  </si>
-  <si>
     <t>&lt;ClientName provided in Client_Config Sheet&gt;</t>
   </si>
   <si>
@@ -452,45 +365,6 @@
     <t xml:space="preserve">Kindly refer to Deployment Document present in docs folder to learn how to use this file </t>
   </si>
   <si>
-    <r>
-      <t>https://</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;TENANTNAME&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.sharepoint.com/sites/</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;CATALOGNAME&gt;</t>
-    </r>
-  </si>
-  <si>
     <t>SiteColumnName</t>
   </si>
   <si>
@@ -558,13 +432,31 @@
   </si>
   <si>
     <t>Contoso,Fabrikam</t>
+  </si>
+  <si>
+    <t>https://M365x102144.sharepoint.com</t>
+  </si>
+  <si>
+    <t>https://M365x102144.sharepoint.com/sites/catalog</t>
+  </si>
+  <si>
+    <t>admin@M365x102144.onmicrosoft.com</t>
+  </si>
+  <si>
+    <t>Microsoft</t>
+  </si>
+  <si>
+    <t>https://M365x102144.sharepoint.com/teams/Microsoft</t>
+  </si>
+  <si>
+    <t>https://M365x102144-admin.sharepoint.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -632,6 +524,14 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -702,10 +602,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -740,9 +641,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -754,8 +652,16 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1067,7 +973,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1080,8 +986,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
-        <v>114</v>
+      <c r="A1" s="16" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1089,7 +995,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1118,11 +1024,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1136,8 +1042,8 @@
       <c r="A1" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>107</v>
+      <c r="B1" s="21" t="s">
+        <v>134</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>45</v>
@@ -1149,7 +1055,7 @@
       </c>
       <c r="B2" s="10" t="str">
         <f>CONCATENATE(B1, "/sites/contentTypeHub")</f>
-        <v>https://&lt;TENANTNAME&gt;.sharepoint.com/sites/contentTypeHub</v>
+        <v>https://M365x102144.sharepoint.com/sites/contentTypeHub</v>
       </c>
       <c r="C2" t="s">
         <v>39</v>
@@ -1159,8 +1065,8 @@
       <c r="A3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>116</v>
+      <c r="B3" s="21" t="s">
+        <v>135</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>38</v>
@@ -1170,8 +1076,8 @@
       <c r="A4" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>108</v>
+      <c r="B4" s="21" t="s">
+        <v>139</v>
       </c>
       <c r="C4" t="s">
         <v>40</v>
@@ -1201,21 +1107,26 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Email Only, Document Only, Both"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{2C5E92D0-6652-4554-AA97-78424B7EF564}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{3CA03FEE-047F-43EF-8FD6-56994A315CFD}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{DF607FD0-76E0-4A1B-825B-0B7A99B17640}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1250,8 +1161,8 @@
       <c r="C2" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="14" t="s">
-        <v>109</v>
+      <c r="D2" s="21" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1264,18 +1175,22 @@
       <c r="C3" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="14" t="s">
-        <v>109</v>
+      <c r="D3" s="21" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{BCB4C5F0-37A8-475D-92BE-EC527894069B}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{419B41E7-8FAC-4B2D-A064-74828BA7AC4F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1335,13 +1250,13 @@
         <v>6</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>6</v>
@@ -1364,13 +1279,13 @@
         <v>7</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>7</v>
@@ -1393,13 +1308,13 @@
         <v>8</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>8</v>
@@ -1422,13 +1337,13 @@
         <v>9</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>9</v>
@@ -1451,13 +1366,13 @@
         <v>11</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>11</v>
@@ -1480,13 +1395,13 @@
         <v>12</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>12</v>
@@ -1509,13 +1424,13 @@
         <v>13</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>13</v>
@@ -1538,13 +1453,13 @@
         <v>14</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>14</v>
@@ -1567,13 +1482,13 @@
         <v>16</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>16</v>
@@ -1596,13 +1511,13 @@
         <v>17</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>17</v>
@@ -1625,13 +1540,13 @@
         <v>19</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>19</v>
@@ -1654,13 +1569,13 @@
         <v>20</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>20</v>
@@ -1679,10 +1594,12 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1710,21 +1627,21 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>111</v>
+        <v>137</v>
       </c>
       <c r="B2" s="15">
         <v>100001</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>109</v>
+      <c r="C2" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1854,16 +1771,21 @@
       <c r="E20" s="15"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{CA1B121D-C15C-404C-BE69-3CD79B0C3F7D}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{A01F987A-2BBE-4621-ACD9-3E943D909D6D}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{3FE9FD8A-62BA-4F4B-88D7-78FEA80F9850}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
@@ -1877,130 +1799,131 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="C2" s="19"/>
+      <c r="D2" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="E2" s="19"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="B3" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="C3" s="19"/>
+      <c r="D3" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3" s="19"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="18" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
+      <c r="B4" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="C4" s="19"/>
+      <c r="D4" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" s="19"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="19" t="s">
+      <c r="B5" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="19"/>
+      <c r="D5" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="E5" s="19"/>
+    </row>
+    <row r="6" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="E2" s="20"/>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
+      <c r="B6" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="C6" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="E3" s="20"/>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
+      <c r="D6" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="E6" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="B4" s="19" t="s">
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="E4" s="20"/>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="19" t="s">
+      <c r="B7" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="C7" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="B5" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="E5" s="20"/>
-    </row>
-    <row r="6" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="19" t="s">
+      <c r="D7" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="E7" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="B6" s="19" t="s">
+    </row>
+    <row r="8" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="B8" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="D6" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="E6" s="19" t="s">
+      <c r="C8" s="18"/>
+      <c r="D8" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="E8" s="18" t="s">
         <v>133</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="19" t="s">
-        <v>134</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="19" t="s">
-        <v>137</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>138</v>
-      </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>139</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2010,7 +1933,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
@@ -2078,7 +2001,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>72</v>
@@ -2125,7 +2048,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B3" t="s">
         <v>73</v>
@@ -2172,7 +2095,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B4" t="s">
         <v>74</v>
@@ -2219,7 +2142,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>77</v>
@@ -2266,7 +2189,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>79</v>
@@ -2313,7 +2236,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>81</v>
@@ -2360,7 +2283,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>83</v>
@@ -2407,7 +2330,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>85</v>
@@ -2454,7 +2377,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>87</v>
@@ -2501,7 +2424,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>89</v>
@@ -2548,7 +2471,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>91</v>
@@ -2595,7 +2518,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>93</v>
@@ -2642,7 +2565,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>95</v>
@@ -2689,7 +2612,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>97</v>
@@ -2736,7 +2659,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>99</v>

</xml_diff>